<commit_message>
Update flapping charts to use Arial as font
Signed-off-by: nook24 <info@nook24.eu>
</commit_message>
<xml_diff>
--- a/src/public/images/usersguide/flapping/statetransitions.xlsx
+++ b/src/public/images/usersguide/flapping/statetransitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8959115F-73FB-4B21-B70C-D32F95782559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32A183A-8310-4270-A7A2-28D201A702AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{375C15B6-4EBF-41E0-A391-26F02FFE1E16}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,7 +160,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -199,20 +199,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1"/>
+              <a:rPr lang="de-DE" sz="1800" b="1" cap="none" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Service State Transitions</a:t>
             </a:r>
           </a:p>
@@ -231,16 +234,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="de-DE"/>
@@ -691,20 +694,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:rPr lang="de-DE" sz="2000" cap="none" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>Time </a:t>
                 </a:r>
               </a:p>
@@ -723,16 +729,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="de-DE"/>
@@ -761,16 +767,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -797,20 +803,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:rPr lang="de-DE" sz="2000" cap="none" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>State</a:t>
                 </a:r>
               </a:p>
@@ -829,16 +838,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="de-DE"/>
@@ -933,16 +942,22 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t>WEIGHTED STATE TRANSITIONS </a:t>
+              <a:rPr lang="de-DE" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Weighted State Transitions </a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE" sz="1800" b="1"/>
+            <a:endParaRPr lang="de-DE" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -966,9 +981,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="de-DE"/>
@@ -1380,9 +1395,9 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -1393,10 +1408,15 @@
                         <a:lumOff val="35000"/>
                       </a:sysClr>
                     </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>TIME</a:t>
+                  <a:t>Time</a:t>
                 </a:r>
-                <a:endParaRPr lang="de-DE" sz="2000"/>
+                <a:endParaRPr lang="de-DE" sz="2000">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1420,9 +1440,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="de-DE"/>
@@ -1458,9 +1478,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -1507,16 +1527,22 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-                  <a:t>WEIGHT</a:t>
+                  <a:rPr lang="de-DE" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Weight</a:t>
                 </a:r>
-                <a:endParaRPr lang="de-DE" sz="2000"/>
+                <a:endParaRPr lang="de-DE" sz="2000">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1540,9 +1566,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="de-DE"/>
@@ -1572,9 +1598,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -1611,6 +1637,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="164282639"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3322,13 +3349,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>383415</xdr:colOff>
+      <xdr:colOff>629947</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>105421</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>273511</xdr:colOff>
+      <xdr:colOff>520043</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>105421</xdr:rowOff>
     </xdr:to>
@@ -3345,7 +3372,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11051415" y="12487921"/>
+          <a:off x="11297947" y="12487921"/>
           <a:ext cx="652096" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3701,7 +3728,7 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>